<commit_message>
change in plan backend
</commit_message>
<xml_diff>
--- a/Project Plan Gantt Chart .xlsx
+++ b/Project Plan Gantt Chart .xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{64EA1721-4985-4386-B9DB-DD5E96E3C344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4826AD09-9CE4-4D04-A8F1-B6654A0750E3}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="8_{64EA1721-4985-4386-B9DB-DD5E96E3C344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C6CFDF1-C3F6-4E75-BC93-3FEA2EF41B9D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -240,12 +240,6 @@
     <t>Implement REST api endpoints</t>
   </si>
   <si>
-    <t xml:space="preserve">Connect react app to spring boot app </t>
-  </si>
-  <si>
-    <t>Fenna &amp; Charlotte/Oisin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Edit Profile page </t>
   </si>
   <si>
@@ -330,12 +324,6 @@
     <t>Create Standard queries for the backend team</t>
   </si>
   <si>
-    <t xml:space="preserve">Connect spring boot backend to database </t>
-  </si>
-  <si>
-    <t>Fenna &amp; Sean/Stephen/Nishant</t>
-  </si>
-  <si>
     <t xml:space="preserve">Model training and testing </t>
   </si>
   <si>
@@ -376,6 +364,12 @@
   </si>
   <si>
     <t>Improve Visualisations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect all parts </t>
+  </si>
+  <si>
+    <t>Deploy spring boot to lambda</t>
   </si>
 </sst>
 </file>
@@ -1407,6 +1401,10 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="38" fillId="41" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1424,10 +1422,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="38" fillId="41" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1830,10 +1824,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2102,9 +2092,9 @@
   </sheetPr>
   <dimension ref="A1:CN61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38:XFD40"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="53" zoomScaleNormal="53" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2125,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -2139,14 +2129,14 @@
     <row r="2" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="36"/>
       <c r="B2" s="73" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="4"/>
       <c r="F2" s="24"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="80" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2155,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I3" s="46"/>
     </row>
@@ -2164,151 +2154,151 @@
         <v>2</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85">
+      <c r="D4" s="86"/>
+      <c r="E4" s="87">
         <v>45201</v>
       </c>
-      <c r="F4" s="85"/>
+      <c r="F4" s="87"/>
     </row>
     <row r="5" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="84"/>
+      <c r="D5" s="86"/>
       <c r="E5" s="7">
         <v>1</v>
       </c>
-      <c r="I5" s="80">
+      <c r="I5" s="82">
         <f>I6</f>
         <v>45201</v>
       </c>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="80">
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="82">
         <f>P6</f>
         <v>45208</v>
       </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="80">
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="82">
         <f>W6</f>
         <v>45215</v>
       </c>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="81"/>
-      <c r="Z5" s="81"/>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="80">
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="82">
         <f>AD6</f>
         <v>45222</v>
       </c>
-      <c r="AE5" s="81"/>
-      <c r="AF5" s="81"/>
-      <c r="AG5" s="81"/>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="80">
+      <c r="AE5" s="83"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="83"/>
+      <c r="AH5" s="83"/>
+      <c r="AI5" s="83"/>
+      <c r="AJ5" s="84"/>
+      <c r="AK5" s="82">
         <f>AK6</f>
         <v>45229</v>
       </c>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="81"/>
-      <c r="AN5" s="81"/>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="80">
+      <c r="AL5" s="83"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="83"/>
+      <c r="AO5" s="83"/>
+      <c r="AP5" s="83"/>
+      <c r="AQ5" s="84"/>
+      <c r="AR5" s="82">
         <f>AR6</f>
         <v>45236</v>
       </c>
-      <c r="AS5" s="81"/>
-      <c r="AT5" s="81"/>
-      <c r="AU5" s="81"/>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="80">
+      <c r="AS5" s="83"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="83"/>
+      <c r="AV5" s="83"/>
+      <c r="AW5" s="83"/>
+      <c r="AX5" s="84"/>
+      <c r="AY5" s="82">
         <f>AY6</f>
         <v>45243</v>
       </c>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="81"/>
-      <c r="BB5" s="81"/>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="80">
+      <c r="AZ5" s="83"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="83"/>
+      <c r="BC5" s="83"/>
+      <c r="BD5" s="83"/>
+      <c r="BE5" s="84"/>
+      <c r="BF5" s="82">
         <f>BF6</f>
         <v>45250</v>
       </c>
-      <c r="BG5" s="81"/>
-      <c r="BH5" s="81"/>
-      <c r="BI5" s="81"/>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="80">
+      <c r="BG5" s="83"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="83"/>
+      <c r="BJ5" s="83"/>
+      <c r="BK5" s="83"/>
+      <c r="BL5" s="84"/>
+      <c r="BM5" s="82">
         <f>BM6</f>
         <v>45257</v>
       </c>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="81"/>
-      <c r="BP5" s="81"/>
-      <c r="BQ5" s="81"/>
-      <c r="BR5" s="81"/>
-      <c r="BS5" s="82"/>
-      <c r="BT5" s="80">
+      <c r="BN5" s="83"/>
+      <c r="BO5" s="83"/>
+      <c r="BP5" s="83"/>
+      <c r="BQ5" s="83"/>
+      <c r="BR5" s="83"/>
+      <c r="BS5" s="84"/>
+      <c r="BT5" s="82">
         <f>BT6</f>
         <v>45264</v>
       </c>
-      <c r="BU5" s="81"/>
-      <c r="BV5" s="81"/>
-      <c r="BW5" s="81"/>
-      <c r="BX5" s="81"/>
-      <c r="BY5" s="81"/>
-      <c r="BZ5" s="82"/>
-      <c r="CA5" s="80">
+      <c r="BU5" s="83"/>
+      <c r="BV5" s="83"/>
+      <c r="BW5" s="83"/>
+      <c r="BX5" s="83"/>
+      <c r="BY5" s="83"/>
+      <c r="BZ5" s="84"/>
+      <c r="CA5" s="82">
         <f>CA6</f>
         <v>45271</v>
       </c>
-      <c r="CB5" s="81"/>
-      <c r="CC5" s="81"/>
-      <c r="CD5" s="81"/>
-      <c r="CE5" s="81"/>
-      <c r="CF5" s="81"/>
-      <c r="CG5" s="82"/>
-      <c r="CH5" s="80">
+      <c r="CB5" s="83"/>
+      <c r="CC5" s="83"/>
+      <c r="CD5" s="83"/>
+      <c r="CE5" s="83"/>
+      <c r="CF5" s="83"/>
+      <c r="CG5" s="84"/>
+      <c r="CH5" s="82">
         <f>CH6</f>
         <v>45278</v>
       </c>
-      <c r="CI5" s="81"/>
-      <c r="CJ5" s="81"/>
-      <c r="CK5" s="81"/>
-      <c r="CL5" s="81"/>
-      <c r="CM5" s="81"/>
-      <c r="CN5" s="82"/>
+      <c r="CI5" s="83"/>
+      <c r="CJ5" s="83"/>
+      <c r="CK5" s="83"/>
+      <c r="CL5" s="83"/>
+      <c r="CM5" s="83"/>
+      <c r="CN5" s="84"/>
     </row>
     <row r="6" spans="1:92" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
@@ -2668,7 +2658,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>19</v>
@@ -3742,13 +3732,13 @@
     </row>
     <row r="15" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="56" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="56" t="s">
-        <v>75</v>
       </c>
       <c r="D15" s="57"/>
       <c r="E15" s="72">
@@ -3850,10 +3840,10 @@
     <row r="16" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="35"/>
       <c r="B16" s="71" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D16" s="57"/>
       <c r="E16" s="72">
@@ -4161,7 +4151,7 @@
     <row r="19" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="35"/>
       <c r="B19" s="66" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="40" t="s">
         <v>51</v>
@@ -4266,7 +4256,7 @@
     <row r="20" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="35"/>
       <c r="B20" s="66" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="40" t="s">
         <v>51</v>
@@ -4367,17 +4357,17 @@
     </row>
     <row r="21" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="35"/>
-      <c r="B21" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="69">
+      <c r="B21" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="57"/>
+      <c r="E21" s="72">
         <v>45208</v>
       </c>
-      <c r="F21" s="69">
+      <c r="F21" s="72">
         <v>45214</v>
       </c>
       <c r="G21" s="14"/>
@@ -4401,7 +4391,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
       <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
+      <c r="Y21" s="22"/>
       <c r="Z21" s="21"/>
       <c r="AA21" s="21"/>
       <c r="AB21" s="21"/>
@@ -4476,7 +4466,7 @@
         <v>76</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22" s="57"/>
       <c r="E22" s="72">
@@ -4506,7 +4496,7 @@
       <c r="V22" s="21"/>
       <c r="W22" s="21"/>
       <c r="X22" s="21"/>
-      <c r="Y22" s="22"/>
+      <c r="Y22" s="21"/>
       <c r="Z22" s="21"/>
       <c r="AA22" s="21"/>
       <c r="AB22" s="21"/>
@@ -4578,10 +4568,10 @@
     <row r="23" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="35"/>
       <c r="B23" s="71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D23" s="57"/>
       <c r="E23" s="72">
@@ -4682,17 +4672,17 @@
     </row>
     <row r="24" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="35"/>
-      <c r="B24" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="72">
+      <c r="B24" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="55"/>
+      <c r="E24" s="69">
         <v>45208</v>
       </c>
-      <c r="F24" s="72">
+      <c r="F24" s="69">
         <v>45214</v>
       </c>
       <c r="G24" s="14"/>
@@ -4786,20 +4776,24 @@
       <c r="CN24" s="21"/>
     </row>
     <row r="25" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="65"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="55"/>
+      <c r="E25" s="69">
+        <v>45208</v>
+      </c>
+      <c r="F25" s="69">
+        <v>45221</v>
+      </c>
       <c r="G25" s="14"/>
-      <c r="H25" s="14" t="str">
+      <c r="H25" s="14">
         <f t="shared" si="32"/>
-        <v/>
+        <v>14</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
@@ -4888,23 +4882,23 @@
     </row>
     <row r="26" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="35"/>
-      <c r="B26" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="67">
-        <v>45215</v>
-      </c>
-      <c r="F26" s="67">
+      <c r="B26" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="75">
+        <v>45208</v>
+      </c>
+      <c r="F26" s="75">
         <v>45221</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14">
         <f t="shared" si="32"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
@@ -4992,24 +4986,20 @@
       <c r="CN26" s="21"/>
     </row>
     <row r="27" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="35"/>
-      <c r="B27" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="67">
-        <v>45215</v>
-      </c>
-      <c r="F27" s="67">
-        <v>45221</v>
-      </c>
+      <c r="A27" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="62"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="65"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="14">
+      <c r="H27" s="14" t="str">
         <f t="shared" si="32"/>
-        <v>7</v>
+        <v/>
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
@@ -5098,17 +5088,17 @@
     </row>
     <row r="28" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="35"/>
-      <c r="B28" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="55"/>
-      <c r="E28" s="69">
+      <c r="B28" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="67">
         <v>45215</v>
       </c>
-      <c r="F28" s="69">
+      <c r="F28" s="67">
         <v>45221</v>
       </c>
       <c r="G28" s="14"/>
@@ -5203,17 +5193,17 @@
     </row>
     <row r="29" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="35"/>
-      <c r="B29" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="55"/>
-      <c r="E29" s="69">
+      <c r="B29" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="67">
         <v>45215</v>
       </c>
-      <c r="F29" s="69">
+      <c r="F29" s="67">
         <v>45221</v>
       </c>
       <c r="G29" s="14"/>
@@ -5309,10 +5299,10 @@
     <row r="30" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="35"/>
       <c r="B30" s="71" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="72">
@@ -5414,10 +5404,10 @@
     <row r="31" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="35"/>
       <c r="B31" s="77" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D31" s="57"/>
       <c r="E31" s="72">
@@ -5519,10 +5509,10 @@
     <row r="32" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="35"/>
       <c r="B32" s="74" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="75">
@@ -5725,10 +5715,10 @@
     <row r="34" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="35"/>
       <c r="B34" s="77" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D34" s="57"/>
       <c r="E34" s="72">
@@ -5830,10 +5820,10 @@
     <row r="35" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="35"/>
       <c r="B35" s="77" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D35" s="57"/>
       <c r="E35" s="72">
@@ -5932,10 +5922,10 @@
     <row r="36" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="35"/>
       <c r="B36" s="78" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="75">
@@ -6034,10 +6024,10 @@
     <row r="37" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="35"/>
       <c r="B37" s="74" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="75">
@@ -6141,7 +6131,7 @@
         <v>11</v>
       </c>
       <c r="B38" s="61" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C38" s="62"/>
       <c r="D38" s="63"/>
@@ -6240,10 +6230,10 @@
     <row r="39" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="35"/>
       <c r="B39" s="77" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D39" s="57"/>
       <c r="E39" s="72">
@@ -6344,11 +6334,11 @@
     </row>
     <row r="40" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="35"/>
-      <c r="B40" s="87" t="s">
-        <v>92</v>
+      <c r="B40" s="81" t="s">
+        <v>88</v>
       </c>
       <c r="C40" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D40" s="57"/>
       <c r="E40" s="72">
@@ -6450,10 +6440,10 @@
     <row r="41" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="35"/>
       <c r="B41" s="77" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D41" s="57"/>
       <c r="E41" s="72">
@@ -6555,10 +6545,10 @@
     <row r="42" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="35"/>
       <c r="B42" s="74" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C42" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="75">
@@ -6660,10 +6650,10 @@
     <row r="43" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="35"/>
       <c r="B43" s="74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C43" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="75">
@@ -6765,10 +6755,10 @@
     <row r="44" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="35"/>
       <c r="B44" s="74" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C44" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="75">
@@ -6872,7 +6862,7 @@
         <v>11</v>
       </c>
       <c r="B45" s="61" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C45" s="62"/>
       <c r="D45" s="63"/>
@@ -6971,10 +6961,10 @@
     <row r="46" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="35"/>
       <c r="B46" s="74" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="75">
@@ -7076,10 +7066,10 @@
     <row r="47" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="35"/>
       <c r="B47" s="74" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="75">
@@ -7181,10 +7171,10 @@
     <row r="48" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="35"/>
       <c r="B48" s="74" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C48" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="75">
@@ -7286,10 +7276,10 @@
     <row r="49" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="35"/>
       <c r="B49" s="71" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C49" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D49" s="57"/>
       <c r="E49" s="72">
@@ -7391,10 +7381,10 @@
     <row r="50" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="35"/>
       <c r="B50" s="71" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C50" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D50" s="57"/>
       <c r="E50" s="72">
@@ -7496,10 +7486,10 @@
     <row r="51" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="35"/>
       <c r="B51" s="71" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C51" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D51" s="57"/>
       <c r="E51" s="72">
@@ -7601,10 +7591,10 @@
     <row r="52" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="35"/>
       <c r="B52" s="71" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C52" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D52" s="57"/>
       <c r="E52" s="72">
@@ -7706,10 +7696,10 @@
     <row r="53" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="35"/>
       <c r="B53" s="74" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C53" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="75">
@@ -7813,7 +7803,7 @@
         <v>11</v>
       </c>
       <c r="B54" s="61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C54" s="62"/>
       <c r="D54" s="63"/>
@@ -7912,10 +7902,10 @@
     <row r="55" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="35"/>
       <c r="B55" s="74" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C55" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="75">
@@ -8017,10 +8007,10 @@
     <row r="56" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="35"/>
       <c r="B56" s="74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C56" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="75">
@@ -8563,15 +8553,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8859,6 +8840,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
@@ -8872,14 +8862,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8898,4 +8880,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Project Plan Gantt Chart .xlsx
</commit_message>
<xml_diff>
--- a/Project Plan Gantt Chart .xlsx
+++ b/Project Plan Gantt Chart .xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="197" documentId="8_{64EA1721-4985-4386-B9DB-DD5E96E3C344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C6CFDF1-C3F6-4E75-BC93-3FEA2EF41B9D}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{64EA1721-4985-4386-B9DB-DD5E96E3C344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50AB580B-3229-4445-A003-0C4019AFCB08}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="0" windowWidth="19600" windowHeight="14410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -198,12 +198,6 @@
     <t xml:space="preserve">Week 4 </t>
   </si>
   <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 6 </t>
-  </si>
-  <si>
     <t>Landing page and homepage layouts</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
     <t xml:space="preserve">Implement map pointer functionality </t>
   </si>
   <si>
-    <t>Buffer Time</t>
-  </si>
-  <si>
     <t>Final Adjustments</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
     <t>Model optimisation and validation</t>
   </si>
   <si>
-    <t xml:space="preserve">Working Prototype </t>
-  </si>
-  <si>
     <t xml:space="preserve">Implement Refactoring </t>
   </si>
   <si>
@@ -370,6 +358,9 @@
   </si>
   <si>
     <t>Deploy spring boot to lambda</t>
+  </si>
+  <si>
+    <t>Week 5 + 6</t>
   </si>
 </sst>
 </file>
@@ -1824,6 +1815,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2090,11 +2085,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CN61"/>
+  <dimension ref="A1:CN58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="53" zoomScaleNormal="53" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2115,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -2129,7 +2124,7 @@
     <row r="2" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="36"/>
       <c r="B2" s="73" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -2145,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I3" s="46"/>
     </row>
@@ -2154,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C4" s="85" t="s">
         <v>16</v>
@@ -2170,7 +2165,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5" s="85" t="s">
         <v>17</v>
@@ -2658,7 +2653,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>19</v>
@@ -3115,7 +3110,7 @@
       <c r="F9" s="65"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="str">
-        <f t="shared" ref="H9:H58" si="32">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H9:H55" si="32">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I9" s="21"/>
@@ -3208,10 +3203,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="67">
@@ -3316,10 +3311,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="67">
@@ -3421,10 +3416,10 @@
     <row r="12" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="35"/>
       <c r="B12" s="66" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="67">
@@ -3526,10 +3521,10 @@
     <row r="13" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="35"/>
       <c r="B13" s="70" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="55"/>
       <c r="E13" s="69">
@@ -3628,10 +3623,10 @@
     <row r="14" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="35"/>
       <c r="B14" s="68" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="55"/>
       <c r="E14" s="69">
@@ -3732,13 +3727,13 @@
     </row>
     <row r="15" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D15" s="57"/>
       <c r="E15" s="72">
@@ -3840,10 +3835,10 @@
     <row r="16" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="35"/>
       <c r="B16" s="71" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D16" s="57"/>
       <c r="E16" s="72">
@@ -4046,10 +4041,10 @@
     <row r="18" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="36"/>
       <c r="B18" s="66" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="67">
@@ -4151,10 +4146,10 @@
     <row r="19" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="35"/>
       <c r="B19" s="66" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="67">
@@ -4256,10 +4251,10 @@
     <row r="20" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="35"/>
       <c r="B20" s="66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="67">
@@ -4358,10 +4353,10 @@
     <row r="21" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="35"/>
       <c r="B21" s="71" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D21" s="57"/>
       <c r="E21" s="72">
@@ -4463,10 +4458,10 @@
     <row r="22" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="35"/>
       <c r="B22" s="71" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D22" s="57"/>
       <c r="E22" s="72">
@@ -4568,10 +4563,10 @@
     <row r="23" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="35"/>
       <c r="B23" s="71" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D23" s="57"/>
       <c r="E23" s="72">
@@ -4673,10 +4668,10 @@
     <row r="24" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="35"/>
       <c r="B24" s="68" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24" s="55"/>
       <c r="E24" s="69">
@@ -4776,24 +4771,20 @@
       <c r="CN24" s="21"/>
     </row>
     <row r="25" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="35"/>
-      <c r="B25" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="69">
-        <v>45208</v>
-      </c>
-      <c r="F25" s="69">
-        <v>45221</v>
-      </c>
+      <c r="A25" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="14">
+      <c r="H25" s="14" t="str">
         <f t="shared" si="32"/>
-        <v>14</v>
+        <v/>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
@@ -4882,23 +4873,23 @@
     </row>
     <row r="26" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="35"/>
-      <c r="B26" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="75">
-        <v>45208</v>
-      </c>
-      <c r="F26" s="75">
+      <c r="B26" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="67">
+        <v>45215</v>
+      </c>
+      <c r="F26" s="67">
         <v>45221</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14">
         <f t="shared" si="32"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
@@ -4986,20 +4977,24 @@
       <c r="CN26" s="21"/>
     </row>
     <row r="27" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="65"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="67">
+        <v>45215</v>
+      </c>
+      <c r="F27" s="67">
+        <v>45221</v>
+      </c>
       <c r="G27" s="14"/>
-      <c r="H27" s="14" t="str">
+      <c r="H27" s="14">
         <f t="shared" si="32"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
@@ -5088,17 +5083,17 @@
     </row>
     <row r="28" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="35"/>
-      <c r="B28" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="67">
+      <c r="B28" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="57"/>
+      <c r="E28" s="72">
         <v>45215</v>
       </c>
-      <c r="F28" s="67">
+      <c r="F28" s="72">
         <v>45221</v>
       </c>
       <c r="G28" s="14"/>
@@ -5193,17 +5188,17 @@
     </row>
     <row r="29" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="35"/>
-      <c r="B29" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="67">
+      <c r="B29" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="57"/>
+      <c r="E29" s="72">
         <v>45215</v>
       </c>
-      <c r="F29" s="67">
+      <c r="F29" s="72">
         <v>45221</v>
       </c>
       <c r="G29" s="14"/>
@@ -5298,23 +5293,23 @@
     </row>
     <row r="30" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="35"/>
-      <c r="B30" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="57"/>
-      <c r="E30" s="72">
-        <v>45215</v>
-      </c>
-      <c r="F30" s="72">
-        <v>45221</v>
+      <c r="B30" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="55"/>
+      <c r="E30" s="69">
+        <v>45208</v>
+      </c>
+      <c r="F30" s="69">
+        <v>45225</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14">
         <f t="shared" si="32"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
@@ -5403,23 +5398,23 @@
     </row>
     <row r="31" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="35"/>
-      <c r="B31" s="77" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="57"/>
-      <c r="E31" s="72">
+      <c r="B31" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="75">
         <v>45215</v>
       </c>
-      <c r="F31" s="72">
-        <v>45221</v>
+      <c r="F31" s="75">
+        <v>45225</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14">
         <f t="shared" si="32"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
@@ -5509,10 +5504,10 @@
     <row r="32" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="35"/>
       <c r="B32" s="74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="75">
@@ -5612,20 +5607,24 @@
       <c r="CN32" s="21"/>
     </row>
     <row r="33" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="65"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="57"/>
+      <c r="E33" s="72">
+        <v>45222</v>
+      </c>
+      <c r="F33" s="72">
+        <v>45228</v>
+      </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="14" t="str">
+      <c r="H33" s="14">
         <f t="shared" si="32"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I33" s="21"/>
       <c r="J33" s="21"/>
@@ -5715,10 +5714,10 @@
     <row r="34" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="35"/>
       <c r="B34" s="77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D34" s="57"/>
       <c r="E34" s="72">
@@ -5728,10 +5727,7 @@
         <v>45228</v>
       </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="14">
-        <f t="shared" si="32"/>
-        <v>7</v>
-      </c>
+      <c r="H34" s="14"/>
       <c r="I34" s="21"/>
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
@@ -5818,22 +5814,21 @@
       <c r="CN34" s="21"/>
     </row>
     <row r="35" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="35"/>
-      <c r="B35" s="77" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="57"/>
-      <c r="E35" s="72">
-        <v>45222</v>
-      </c>
-      <c r="F35" s="72">
-        <v>45228</v>
-      </c>
+      <c r="A35" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="62"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="H35" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
       <c r="I35" s="21"/>
       <c r="J35" s="21"/>
       <c r="K35" s="21"/>
@@ -5921,21 +5916,24 @@
     </row>
     <row r="36" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="35"/>
-      <c r="B36" s="78" t="s">
+      <c r="B36" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="75">
-        <v>45222</v>
-      </c>
-      <c r="F36" s="75">
-        <v>45225</v>
+      <c r="C36" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="57"/>
+      <c r="E36" s="72">
+        <v>45227</v>
+      </c>
+      <c r="F36" s="72">
+        <v>45242</v>
       </c>
       <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
+      <c r="H36" s="14">
+        <f t="shared" si="32"/>
+        <v>16</v>
+      </c>
       <c r="I36" s="21"/>
       <c r="J36" s="21"/>
       <c r="K36" s="21"/>
@@ -6023,23 +6021,23 @@
     </row>
     <row r="37" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="35"/>
-      <c r="B37" s="74" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="75">
-        <v>45222</v>
-      </c>
-      <c r="F37" s="75">
-        <v>45225</v>
+      <c r="B37" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="57"/>
+      <c r="E37" s="72">
+        <v>45227</v>
+      </c>
+      <c r="F37" s="72">
+        <v>45242</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="14">
         <f t="shared" si="32"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
@@ -6127,20 +6125,24 @@
       <c r="CN37" s="21"/>
     </row>
     <row r="38" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="65"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="57"/>
+      <c r="E38" s="72">
+        <v>45227</v>
+      </c>
+      <c r="F38" s="72">
+        <v>45242</v>
+      </c>
       <c r="G38" s="14"/>
-      <c r="H38" s="14" t="str">
+      <c r="H38" s="14">
         <f t="shared" si="32"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="I38" s="21"/>
       <c r="J38" s="21"/>
@@ -6229,17 +6231,17 @@
     </row>
     <row r="39" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="35"/>
-      <c r="B39" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="57"/>
-      <c r="E39" s="72">
+      <c r="B39" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="E39" s="75">
         <v>45227</v>
       </c>
-      <c r="F39" s="72">
+      <c r="F39" s="75">
         <v>45242</v>
       </c>
       <c r="G39" s="14"/>
@@ -6334,17 +6336,17 @@
     </row>
     <row r="40" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="35"/>
-      <c r="B40" s="81" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="57"/>
-      <c r="E40" s="72">
+      <c r="B40" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="75">
         <v>45227</v>
       </c>
-      <c r="F40" s="72">
+      <c r="F40" s="75">
         <v>45242</v>
       </c>
       <c r="G40" s="14"/>
@@ -6439,17 +6441,17 @@
     </row>
     <row r="41" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="35"/>
-      <c r="B41" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="57"/>
-      <c r="E41" s="72">
+      <c r="B41" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="75">
         <v>45227</v>
       </c>
-      <c r="F41" s="72">
+      <c r="F41" s="75">
         <v>45242</v>
       </c>
       <c r="G41" s="14"/>
@@ -6543,24 +6545,20 @@
       <c r="CN41" s="21"/>
     </row>
     <row r="42" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="35"/>
-      <c r="B42" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="75">
-        <v>45227</v>
-      </c>
-      <c r="F42" s="75">
-        <v>45242</v>
-      </c>
+      <c r="A42" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="62"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="65"/>
       <c r="G42" s="14"/>
-      <c r="H42" s="14">
+      <c r="H42" s="14" t="str">
         <f t="shared" si="32"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="I42" s="21"/>
       <c r="J42" s="21"/>
@@ -6650,22 +6648,22 @@
     <row r="43" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="35"/>
       <c r="B43" s="74" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C43" s="41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="75">
-        <v>45227</v>
+        <v>45243</v>
       </c>
       <c r="F43" s="75">
-        <v>45242</v>
+        <v>45246</v>
       </c>
       <c r="G43" s="14"/>
       <c r="H43" s="14">
         <f t="shared" si="32"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
@@ -6755,22 +6753,22 @@
     <row r="44" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="35"/>
       <c r="B44" s="74" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C44" s="41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="75">
-        <v>45227</v>
+        <v>45243</v>
       </c>
       <c r="F44" s="75">
-        <v>45242</v>
+        <v>45256</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14">
         <f t="shared" si="32"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="21"/>
@@ -6820,7 +6818,7 @@
       <c r="BB44" s="21"/>
       <c r="BC44" s="21"/>
       <c r="BD44" s="21"/>
-      <c r="BE44" s="21"/>
+      <c r="BE44" s="79"/>
       <c r="BF44" s="21"/>
       <c r="BG44" s="21"/>
       <c r="BH44" s="21"/>
@@ -6858,20 +6856,24 @@
       <c r="CN44" s="21"/>
     </row>
     <row r="45" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="62"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="65"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="75">
+        <v>45243</v>
+      </c>
+      <c r="F45" s="75">
+        <v>45256</v>
+      </c>
       <c r="G45" s="14"/>
-      <c r="H45" s="14" t="str">
+      <c r="H45" s="14">
         <f t="shared" si="32"/>
-        <v/>
+        <v>14</v>
       </c>
       <c r="I45" s="21"/>
       <c r="J45" s="21"/>
@@ -6921,7 +6923,7 @@
       <c r="BB45" s="21"/>
       <c r="BC45" s="21"/>
       <c r="BD45" s="21"/>
-      <c r="BE45" s="21"/>
+      <c r="BE45" s="79"/>
       <c r="BF45" s="21"/>
       <c r="BG45" s="21"/>
       <c r="BH45" s="21"/>
@@ -6960,23 +6962,23 @@
     </row>
     <row r="46" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="35"/>
-      <c r="B46" s="74" t="s">
+      <c r="B46" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="16"/>
-      <c r="E46" s="75">
+      <c r="C46" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="57"/>
+      <c r="E46" s="72">
         <v>45243</v>
       </c>
-      <c r="F46" s="75">
-        <v>45246</v>
+      <c r="F46" s="72">
+        <v>45270</v>
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="14">
         <f t="shared" si="32"/>
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
@@ -7026,21 +7028,21 @@
       <c r="BB46" s="21"/>
       <c r="BC46" s="21"/>
       <c r="BD46" s="21"/>
-      <c r="BE46" s="21"/>
+      <c r="BE46" s="79"/>
       <c r="BF46" s="21"/>
       <c r="BG46" s="21"/>
       <c r="BH46" s="21"/>
       <c r="BI46" s="21"/>
       <c r="BJ46" s="21"/>
       <c r="BK46" s="21"/>
-      <c r="BL46" s="21"/>
-      <c r="BM46" s="21"/>
+      <c r="BL46" s="79"/>
+      <c r="BM46" s="79"/>
       <c r="BN46" s="21"/>
       <c r="BO46" s="21"/>
       <c r="BP46" s="21"/>
       <c r="BQ46" s="21"/>
       <c r="BR46" s="21"/>
-      <c r="BS46" s="21"/>
+      <c r="BS46" s="79"/>
       <c r="BT46" s="21"/>
       <c r="BU46" s="21"/>
       <c r="BV46" s="21"/>
@@ -7065,23 +7067,23 @@
     </row>
     <row r="47" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="35"/>
-      <c r="B47" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="75">
+      <c r="B47" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="57"/>
+      <c r="E47" s="72">
         <v>45243</v>
       </c>
-      <c r="F47" s="75">
-        <v>45256</v>
+      <c r="F47" s="72">
+        <v>45270</v>
       </c>
       <c r="G47" s="14"/>
       <c r="H47" s="14">
         <f t="shared" si="32"/>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I47" s="21"/>
       <c r="J47" s="21"/>
@@ -7138,14 +7140,14 @@
       <c r="BI47" s="21"/>
       <c r="BJ47" s="21"/>
       <c r="BK47" s="21"/>
-      <c r="BL47" s="21"/>
+      <c r="BL47" s="79"/>
       <c r="BM47" s="21"/>
       <c r="BN47" s="21"/>
       <c r="BO47" s="21"/>
       <c r="BP47" s="21"/>
       <c r="BQ47" s="21"/>
       <c r="BR47" s="21"/>
-      <c r="BS47" s="21"/>
+      <c r="BS47" s="79"/>
       <c r="BT47" s="21"/>
       <c r="BU47" s="21"/>
       <c r="BV47" s="21"/>
@@ -7170,23 +7172,23 @@
     </row>
     <row r="48" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="35"/>
-      <c r="B48" s="74" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="75">
+      <c r="B48" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="57"/>
+      <c r="E48" s="72">
         <v>45243</v>
       </c>
-      <c r="F48" s="75">
-        <v>45256</v>
+      <c r="F48" s="72">
+        <v>45270</v>
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="14">
         <f t="shared" si="32"/>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I48" s="21"/>
       <c r="J48" s="21"/>
@@ -7243,14 +7245,14 @@
       <c r="BI48" s="21"/>
       <c r="BJ48" s="21"/>
       <c r="BK48" s="21"/>
-      <c r="BL48" s="21"/>
+      <c r="BL48" s="79"/>
       <c r="BM48" s="21"/>
       <c r="BN48" s="21"/>
       <c r="BO48" s="21"/>
       <c r="BP48" s="21"/>
       <c r="BQ48" s="21"/>
       <c r="BR48" s="21"/>
-      <c r="BS48" s="21"/>
+      <c r="BS48" s="79"/>
       <c r="BT48" s="21"/>
       <c r="BU48" s="21"/>
       <c r="BV48" s="21"/>
@@ -7276,10 +7278,10 @@
     <row r="49" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="35"/>
       <c r="B49" s="71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" s="56" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D49" s="57"/>
       <c r="E49" s="72">
@@ -7349,7 +7351,7 @@
       <c r="BJ49" s="21"/>
       <c r="BK49" s="21"/>
       <c r="BL49" s="79"/>
-      <c r="BM49" s="79"/>
+      <c r="BM49" s="21"/>
       <c r="BN49" s="21"/>
       <c r="BO49" s="21"/>
       <c r="BP49" s="21"/>
@@ -7380,23 +7382,23 @@
     </row>
     <row r="50" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="35"/>
-      <c r="B50" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" s="57"/>
-      <c r="E50" s="72">
-        <v>45243</v>
-      </c>
-      <c r="F50" s="72">
+      <c r="B50" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="16"/>
+      <c r="E50" s="75">
+        <v>45257</v>
+      </c>
+      <c r="F50" s="75">
         <v>45270</v>
       </c>
       <c r="G50" s="14"/>
       <c r="H50" s="14">
         <f t="shared" si="32"/>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I50" s="21"/>
       <c r="J50" s="21"/>
@@ -7446,14 +7448,14 @@
       <c r="BB50" s="21"/>
       <c r="BC50" s="21"/>
       <c r="BD50" s="21"/>
-      <c r="BE50" s="79"/>
+      <c r="BE50" s="21"/>
       <c r="BF50" s="21"/>
       <c r="BG50" s="21"/>
       <c r="BH50" s="21"/>
       <c r="BI50" s="21"/>
       <c r="BJ50" s="21"/>
       <c r="BK50" s="21"/>
-      <c r="BL50" s="79"/>
+      <c r="BL50" s="21"/>
       <c r="BM50" s="21"/>
       <c r="BN50" s="21"/>
       <c r="BO50" s="21"/>
@@ -7484,24 +7486,20 @@
       <c r="CN50" s="21"/>
     </row>
     <row r="51" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="35"/>
-      <c r="B51" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" s="57"/>
-      <c r="E51" s="72">
-        <v>45243</v>
-      </c>
-      <c r="F51" s="72">
-        <v>45270</v>
-      </c>
+      <c r="A51" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="62"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="65"/>
       <c r="G51" s="14"/>
-      <c r="H51" s="14">
+      <c r="H51" s="14" t="str">
         <f t="shared" si="32"/>
-        <v>28</v>
+        <v/>
       </c>
       <c r="I51" s="21"/>
       <c r="J51" s="21"/>
@@ -7551,21 +7549,21 @@
       <c r="BB51" s="21"/>
       <c r="BC51" s="21"/>
       <c r="BD51" s="21"/>
-      <c r="BE51" s="79"/>
+      <c r="BE51" s="21"/>
       <c r="BF51" s="21"/>
       <c r="BG51" s="21"/>
       <c r="BH51" s="21"/>
       <c r="BI51" s="21"/>
       <c r="BJ51" s="21"/>
       <c r="BK51" s="21"/>
-      <c r="BL51" s="79"/>
+      <c r="BL51" s="21"/>
       <c r="BM51" s="21"/>
       <c r="BN51" s="21"/>
       <c r="BO51" s="21"/>
       <c r="BP51" s="21"/>
       <c r="BQ51" s="21"/>
       <c r="BR51" s="21"/>
-      <c r="BS51" s="79"/>
+      <c r="BS51" s="21"/>
       <c r="BT51" s="21"/>
       <c r="BU51" s="21"/>
       <c r="BV51" s="21"/>
@@ -7590,23 +7588,23 @@
     </row>
     <row r="52" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="35"/>
-      <c r="B52" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" s="57"/>
-      <c r="E52" s="72">
-        <v>45243</v>
-      </c>
-      <c r="F52" s="72">
-        <v>45270</v>
+      <c r="B52" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="16"/>
+      <c r="E52" s="75">
+        <v>45264</v>
+      </c>
+      <c r="F52" s="75">
+        <v>45281</v>
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="14">
         <f t="shared" si="32"/>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I52" s="21"/>
       <c r="J52" s="21"/>
@@ -7656,35 +7654,35 @@
       <c r="BB52" s="21"/>
       <c r="BC52" s="21"/>
       <c r="BD52" s="21"/>
-      <c r="BE52" s="79"/>
+      <c r="BE52" s="21"/>
       <c r="BF52" s="21"/>
       <c r="BG52" s="21"/>
       <c r="BH52" s="21"/>
       <c r="BI52" s="21"/>
       <c r="BJ52" s="21"/>
       <c r="BK52" s="21"/>
-      <c r="BL52" s="79"/>
+      <c r="BL52" s="21"/>
       <c r="BM52" s="21"/>
       <c r="BN52" s="21"/>
       <c r="BO52" s="21"/>
       <c r="BP52" s="21"/>
       <c r="BQ52" s="21"/>
       <c r="BR52" s="21"/>
-      <c r="BS52" s="79"/>
+      <c r="BS52" s="21"/>
       <c r="BT52" s="21"/>
       <c r="BU52" s="21"/>
       <c r="BV52" s="21"/>
       <c r="BW52" s="21"/>
       <c r="BX52" s="21"/>
       <c r="BY52" s="21"/>
-      <c r="BZ52" s="21"/>
+      <c r="BZ52" s="79"/>
       <c r="CA52" s="21"/>
       <c r="CB52" s="21"/>
       <c r="CC52" s="21"/>
       <c r="CD52" s="21"/>
       <c r="CE52" s="21"/>
       <c r="CF52" s="21"/>
-      <c r="CG52" s="21"/>
+      <c r="CG52" s="79"/>
       <c r="CH52" s="21"/>
       <c r="CI52" s="21"/>
       <c r="CJ52" s="21"/>
@@ -7699,19 +7697,19 @@
         <v>62</v>
       </c>
       <c r="C53" s="41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="75">
-        <v>45257</v>
+        <v>45264</v>
       </c>
       <c r="F53" s="75">
-        <v>45270</v>
+        <v>45281</v>
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="14">
         <f t="shared" si="32"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I53" s="21"/>
       <c r="J53" s="21"/>
@@ -7775,21 +7773,21 @@
       <c r="BP53" s="21"/>
       <c r="BQ53" s="21"/>
       <c r="BR53" s="21"/>
-      <c r="BS53" s="79"/>
+      <c r="BS53" s="21"/>
       <c r="BT53" s="21"/>
       <c r="BU53" s="21"/>
       <c r="BV53" s="21"/>
       <c r="BW53" s="21"/>
       <c r="BX53" s="21"/>
       <c r="BY53" s="21"/>
-      <c r="BZ53" s="21"/>
+      <c r="BZ53" s="79"/>
       <c r="CA53" s="21"/>
       <c r="CB53" s="21"/>
       <c r="CC53" s="21"/>
       <c r="CD53" s="21"/>
       <c r="CE53" s="21"/>
       <c r="CF53" s="21"/>
-      <c r="CG53" s="21"/>
+      <c r="CG53" s="79"/>
       <c r="CH53" s="21"/>
       <c r="CI53" s="21"/>
       <c r="CJ53" s="21"/>
@@ -7800,15 +7798,13 @@
     </row>
     <row r="54" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="62"/>
-      <c r="D54" s="63"/>
-      <c r="E54" s="64"/>
-      <c r="F54" s="65"/>
+        <v>12</v>
+      </c>
+      <c r="B54" s="43"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
       <c r="G54" s="14"/>
       <c r="H54" s="14" t="str">
         <f t="shared" si="32"/>
@@ -7900,424 +7896,115 @@
       <c r="CN54" s="21"/>
     </row>
     <row r="55" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="35"/>
-      <c r="B55" s="74" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="16"/>
-      <c r="E55" s="75">
-        <v>45264</v>
-      </c>
-      <c r="F55" s="75">
-        <v>45281</v>
-      </c>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14">
-        <f t="shared" si="32"/>
-        <v>18</v>
-      </c>
-      <c r="I55" s="21"/>
-      <c r="J55" s="21"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="21"/>
-      <c r="M55" s="21"/>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
-      <c r="Q55" s="21"/>
-      <c r="R55" s="21"/>
-      <c r="S55" s="21"/>
-      <c r="T55" s="21"/>
-      <c r="U55" s="21"/>
-      <c r="V55" s="21"/>
-      <c r="W55" s="21"/>
-      <c r="X55" s="21"/>
-      <c r="Y55" s="21"/>
-      <c r="Z55" s="21"/>
-      <c r="AA55" s="21"/>
-      <c r="AB55" s="21"/>
-      <c r="AC55" s="21"/>
-      <c r="AD55" s="21"/>
-      <c r="AE55" s="21"/>
-      <c r="AF55" s="21"/>
-      <c r="AG55" s="21"/>
-      <c r="AH55" s="21"/>
-      <c r="AI55" s="21"/>
-      <c r="AJ55" s="21"/>
-      <c r="AK55" s="21"/>
-      <c r="AL55" s="21"/>
-      <c r="AM55" s="21"/>
-      <c r="AN55" s="21"/>
-      <c r="AO55" s="21"/>
-      <c r="AP55" s="21"/>
-      <c r="AQ55" s="21"/>
-      <c r="AR55" s="21"/>
-      <c r="AS55" s="21"/>
-      <c r="AT55" s="21"/>
-      <c r="AU55" s="21"/>
-      <c r="AV55" s="21"/>
-      <c r="AW55" s="21"/>
-      <c r="AX55" s="21"/>
-      <c r="AY55" s="21"/>
-      <c r="AZ55" s="21"/>
-      <c r="BA55" s="21"/>
-      <c r="BB55" s="21"/>
-      <c r="BC55" s="21"/>
-      <c r="BD55" s="21"/>
-      <c r="BE55" s="21"/>
-      <c r="BF55" s="21"/>
-      <c r="BG55" s="21"/>
-      <c r="BH55" s="21"/>
-      <c r="BI55" s="21"/>
-      <c r="BJ55" s="21"/>
-      <c r="BK55" s="21"/>
-      <c r="BL55" s="21"/>
-      <c r="BM55" s="21"/>
-      <c r="BN55" s="21"/>
-      <c r="BO55" s="21"/>
-      <c r="BP55" s="21"/>
-      <c r="BQ55" s="21"/>
-      <c r="BR55" s="21"/>
-      <c r="BS55" s="21"/>
-      <c r="BT55" s="21"/>
-      <c r="BU55" s="21"/>
-      <c r="BV55" s="21"/>
-      <c r="BW55" s="21"/>
-      <c r="BX55" s="21"/>
-      <c r="BY55" s="21"/>
-      <c r="BZ55" s="79"/>
-      <c r="CA55" s="21"/>
-      <c r="CB55" s="21"/>
-      <c r="CC55" s="21"/>
-      <c r="CD55" s="21"/>
-      <c r="CE55" s="21"/>
-      <c r="CF55" s="21"/>
-      <c r="CG55" s="79"/>
-      <c r="CH55" s="21"/>
-      <c r="CI55" s="21"/>
-      <c r="CJ55" s="21"/>
-      <c r="CK55" s="21"/>
-      <c r="CL55" s="21"/>
-      <c r="CM55" s="21"/>
-      <c r="CN55" s="21"/>
-    </row>
-    <row r="56" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="35"/>
-      <c r="B56" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="75">
-        <v>45264</v>
-      </c>
-      <c r="F56" s="75">
-        <v>45281</v>
-      </c>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14">
-        <f t="shared" si="32"/>
-        <v>18</v>
-      </c>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="21"/>
-      <c r="S56" s="21"/>
-      <c r="T56" s="21"/>
-      <c r="U56" s="21"/>
-      <c r="V56" s="21"/>
-      <c r="W56" s="21"/>
-      <c r="X56" s="21"/>
-      <c r="Y56" s="21"/>
-      <c r="Z56" s="21"/>
-      <c r="AA56" s="21"/>
-      <c r="AB56" s="21"/>
-      <c r="AC56" s="21"/>
-      <c r="AD56" s="21"/>
-      <c r="AE56" s="21"/>
-      <c r="AF56" s="21"/>
-      <c r="AG56" s="21"/>
-      <c r="AH56" s="21"/>
-      <c r="AI56" s="21"/>
-      <c r="AJ56" s="21"/>
-      <c r="AK56" s="21"/>
-      <c r="AL56" s="21"/>
-      <c r="AM56" s="21"/>
-      <c r="AN56" s="21"/>
-      <c r="AO56" s="21"/>
-      <c r="AP56" s="21"/>
-      <c r="AQ56" s="21"/>
-      <c r="AR56" s="21"/>
-      <c r="AS56" s="21"/>
-      <c r="AT56" s="21"/>
-      <c r="AU56" s="21"/>
-      <c r="AV56" s="21"/>
-      <c r="AW56" s="21"/>
-      <c r="AX56" s="21"/>
-      <c r="AY56" s="21"/>
-      <c r="AZ56" s="21"/>
-      <c r="BA56" s="21"/>
-      <c r="BB56" s="21"/>
-      <c r="BC56" s="21"/>
-      <c r="BD56" s="21"/>
-      <c r="BE56" s="21"/>
-      <c r="BF56" s="21"/>
-      <c r="BG56" s="21"/>
-      <c r="BH56" s="21"/>
-      <c r="BI56" s="21"/>
-      <c r="BJ56" s="21"/>
-      <c r="BK56" s="21"/>
-      <c r="BL56" s="21"/>
-      <c r="BM56" s="21"/>
-      <c r="BN56" s="21"/>
-      <c r="BO56" s="21"/>
-      <c r="BP56" s="21"/>
-      <c r="BQ56" s="21"/>
-      <c r="BR56" s="21"/>
-      <c r="BS56" s="21"/>
-      <c r="BT56" s="21"/>
-      <c r="BU56" s="21"/>
-      <c r="BV56" s="21"/>
-      <c r="BW56" s="21"/>
-      <c r="BX56" s="21"/>
-      <c r="BY56" s="21"/>
-      <c r="BZ56" s="79"/>
-      <c r="CA56" s="21"/>
-      <c r="CB56" s="21"/>
-      <c r="CC56" s="21"/>
-      <c r="CD56" s="21"/>
-      <c r="CE56" s="21"/>
-      <c r="CF56" s="21"/>
-      <c r="CG56" s="79"/>
-      <c r="CH56" s="21"/>
-      <c r="CI56" s="21"/>
-      <c r="CJ56" s="21"/>
-      <c r="CK56" s="21"/>
-      <c r="CL56" s="21"/>
-      <c r="CM56" s="21"/>
-      <c r="CN56" s="21"/>
-    </row>
-    <row r="57" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B57" s="43"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14" t="str">
+      <c r="A55" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20" t="str">
         <f t="shared" si="32"/>
         <v/>
       </c>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="21"/>
-      <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
-      <c r="Q57" s="21"/>
-      <c r="R57" s="21"/>
-      <c r="S57" s="21"/>
-      <c r="T57" s="21"/>
-      <c r="U57" s="21"/>
-      <c r="V57" s="21"/>
-      <c r="W57" s="21"/>
-      <c r="X57" s="21"/>
-      <c r="Y57" s="21"/>
-      <c r="Z57" s="21"/>
-      <c r="AA57" s="21"/>
-      <c r="AB57" s="21"/>
-      <c r="AC57" s="21"/>
-      <c r="AD57" s="21"/>
-      <c r="AE57" s="21"/>
-      <c r="AF57" s="21"/>
-      <c r="AG57" s="21"/>
-      <c r="AH57" s="21"/>
-      <c r="AI57" s="21"/>
-      <c r="AJ57" s="21"/>
-      <c r="AK57" s="21"/>
-      <c r="AL57" s="21"/>
-      <c r="AM57" s="21"/>
-      <c r="AN57" s="21"/>
-      <c r="AO57" s="21"/>
-      <c r="AP57" s="21"/>
-      <c r="AQ57" s="21"/>
-      <c r="AR57" s="21"/>
-      <c r="AS57" s="21"/>
-      <c r="AT57" s="21"/>
-      <c r="AU57" s="21"/>
-      <c r="AV57" s="21"/>
-      <c r="AW57" s="21"/>
-      <c r="AX57" s="21"/>
-      <c r="AY57" s="21"/>
-      <c r="AZ57" s="21"/>
-      <c r="BA57" s="21"/>
-      <c r="BB57" s="21"/>
-      <c r="BC57" s="21"/>
-      <c r="BD57" s="21"/>
-      <c r="BE57" s="21"/>
-      <c r="BF57" s="21"/>
-      <c r="BG57" s="21"/>
-      <c r="BH57" s="21"/>
-      <c r="BI57" s="21"/>
-      <c r="BJ57" s="21"/>
-      <c r="BK57" s="21"/>
-      <c r="BL57" s="21"/>
-      <c r="BM57" s="21"/>
-      <c r="BN57" s="21"/>
-      <c r="BO57" s="21"/>
-      <c r="BP57" s="21"/>
-      <c r="BQ57" s="21"/>
-      <c r="BR57" s="21"/>
-      <c r="BS57" s="21"/>
-      <c r="BT57" s="21"/>
-      <c r="BU57" s="21"/>
-      <c r="BV57" s="21"/>
-      <c r="BW57" s="21"/>
-      <c r="BX57" s="21"/>
-      <c r="BY57" s="21"/>
-      <c r="BZ57" s="21"/>
-      <c r="CA57" s="21"/>
-      <c r="CB57" s="21"/>
-      <c r="CC57" s="21"/>
-      <c r="CD57" s="21"/>
-      <c r="CE57" s="21"/>
-      <c r="CF57" s="21"/>
-      <c r="CG57" s="21"/>
-      <c r="CH57" s="21"/>
-      <c r="CI57" s="21"/>
-      <c r="CJ57" s="21"/>
-      <c r="CK57" s="21"/>
-      <c r="CL57" s="21"/>
-      <c r="CM57" s="21"/>
-      <c r="CN57" s="21"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="23"/>
+      <c r="N55" s="23"/>
+      <c r="O55" s="23"/>
+      <c r="P55" s="23"/>
+      <c r="Q55" s="23"/>
+      <c r="R55" s="23"/>
+      <c r="S55" s="23"/>
+      <c r="T55" s="23"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="23"/>
+      <c r="W55" s="23"/>
+      <c r="X55" s="23"/>
+      <c r="Y55" s="23"/>
+      <c r="Z55" s="23"/>
+      <c r="AA55" s="23"/>
+      <c r="AB55" s="23"/>
+      <c r="AC55" s="23"/>
+      <c r="AD55" s="23"/>
+      <c r="AE55" s="23"/>
+      <c r="AF55" s="23"/>
+      <c r="AG55" s="23"/>
+      <c r="AH55" s="23"/>
+      <c r="AI55" s="23"/>
+      <c r="AJ55" s="23"/>
+      <c r="AK55" s="23"/>
+      <c r="AL55" s="23"/>
+      <c r="AM55" s="23"/>
+      <c r="AN55" s="23"/>
+      <c r="AO55" s="23"/>
+      <c r="AP55" s="23"/>
+      <c r="AQ55" s="23"/>
+      <c r="AR55" s="23"/>
+      <c r="AS55" s="23"/>
+      <c r="AT55" s="23"/>
+      <c r="AU55" s="23"/>
+      <c r="AV55" s="23"/>
+      <c r="AW55" s="23"/>
+      <c r="AX55" s="23"/>
+      <c r="AY55" s="23"/>
+      <c r="AZ55" s="23"/>
+      <c r="BA55" s="23"/>
+      <c r="BB55" s="23"/>
+      <c r="BC55" s="23"/>
+      <c r="BD55" s="23"/>
+      <c r="BE55" s="23"/>
+      <c r="BF55" s="23"/>
+      <c r="BG55" s="23"/>
+      <c r="BH55" s="23"/>
+      <c r="BI55" s="23"/>
+      <c r="BJ55" s="23"/>
+      <c r="BK55" s="23"/>
+      <c r="BL55" s="23"/>
+      <c r="BM55" s="23"/>
+      <c r="BN55" s="23"/>
+      <c r="BO55" s="23"/>
+      <c r="BP55" s="23"/>
+      <c r="BQ55" s="23"/>
+      <c r="BR55" s="23"/>
+      <c r="BS55" s="23"/>
+      <c r="BT55" s="23"/>
+      <c r="BU55" s="23"/>
+      <c r="BV55" s="23"/>
+      <c r="BW55" s="23"/>
+      <c r="BX55" s="23"/>
+      <c r="BY55" s="23"/>
+      <c r="BZ55" s="23"/>
+      <c r="CA55" s="23"/>
+      <c r="CB55" s="23"/>
+      <c r="CC55" s="23"/>
+      <c r="CD55" s="23"/>
+      <c r="CE55" s="23"/>
+      <c r="CF55" s="23"/>
+      <c r="CG55" s="23"/>
+      <c r="CH55" s="23"/>
+      <c r="CI55" s="23"/>
+      <c r="CJ55" s="23"/>
+      <c r="CK55" s="23"/>
+      <c r="CL55" s="23"/>
+      <c r="CM55" s="23"/>
+      <c r="CN55" s="23"/>
     </row>
-    <row r="58" spans="1:92" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20" t="str">
-        <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23"/>
-      <c r="K58" s="23"/>
-      <c r="L58" s="23"/>
-      <c r="M58" s="23"/>
-      <c r="N58" s="23"/>
-      <c r="O58" s="23"/>
-      <c r="P58" s="23"/>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="23"/>
-      <c r="S58" s="23"/>
-      <c r="T58" s="23"/>
-      <c r="U58" s="23"/>
-      <c r="V58" s="23"/>
-      <c r="W58" s="23"/>
-      <c r="X58" s="23"/>
-      <c r="Y58" s="23"/>
-      <c r="Z58" s="23"/>
-      <c r="AA58" s="23"/>
-      <c r="AB58" s="23"/>
-      <c r="AC58" s="23"/>
-      <c r="AD58" s="23"/>
-      <c r="AE58" s="23"/>
-      <c r="AF58" s="23"/>
-      <c r="AG58" s="23"/>
-      <c r="AH58" s="23"/>
-      <c r="AI58" s="23"/>
-      <c r="AJ58" s="23"/>
-      <c r="AK58" s="23"/>
-      <c r="AL58" s="23"/>
-      <c r="AM58" s="23"/>
-      <c r="AN58" s="23"/>
-      <c r="AO58" s="23"/>
-      <c r="AP58" s="23"/>
-      <c r="AQ58" s="23"/>
-      <c r="AR58" s="23"/>
-      <c r="AS58" s="23"/>
-      <c r="AT58" s="23"/>
-      <c r="AU58" s="23"/>
-      <c r="AV58" s="23"/>
-      <c r="AW58" s="23"/>
-      <c r="AX58" s="23"/>
-      <c r="AY58" s="23"/>
-      <c r="AZ58" s="23"/>
-      <c r="BA58" s="23"/>
-      <c r="BB58" s="23"/>
-      <c r="BC58" s="23"/>
-      <c r="BD58" s="23"/>
-      <c r="BE58" s="23"/>
-      <c r="BF58" s="23"/>
-      <c r="BG58" s="23"/>
-      <c r="BH58" s="23"/>
-      <c r="BI58" s="23"/>
-      <c r="BJ58" s="23"/>
-      <c r="BK58" s="23"/>
-      <c r="BL58" s="23"/>
-      <c r="BM58" s="23"/>
-      <c r="BN58" s="23"/>
-      <c r="BO58" s="23"/>
-      <c r="BP58" s="23"/>
-      <c r="BQ58" s="23"/>
-      <c r="BR58" s="23"/>
-      <c r="BS58" s="23"/>
-      <c r="BT58" s="23"/>
-      <c r="BU58" s="23"/>
-      <c r="BV58" s="23"/>
-      <c r="BW58" s="23"/>
-      <c r="BX58" s="23"/>
-      <c r="BY58" s="23"/>
-      <c r="BZ58" s="23"/>
-      <c r="CA58" s="23"/>
-      <c r="CB58" s="23"/>
-      <c r="CC58" s="23"/>
-      <c r="CD58" s="23"/>
-      <c r="CE58" s="23"/>
-      <c r="CF58" s="23"/>
-      <c r="CG58" s="23"/>
-      <c r="CH58" s="23"/>
-      <c r="CI58" s="23"/>
-      <c r="CJ58" s="23"/>
-      <c r="CK58" s="23"/>
-      <c r="CL58" s="23"/>
-      <c r="CM58" s="23"/>
-      <c r="CN58" s="23"/>
+    <row r="56" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G56" s="6"/>
     </row>
-    <row r="59" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G59" s="6"/>
+    <row r="57" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C57" s="11"/>
+      <c r="F57" s="37"/>
     </row>
-    <row r="60" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C60" s="11"/>
-      <c r="F60" s="37"/>
-    </row>
-    <row r="61" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C61" s="12"/>
+    <row r="58" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C58" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -8337,7 +8024,7 @@
     <mergeCell ref="W5:AC5"/>
     <mergeCell ref="AD5:AJ5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D8:D58">
+  <conditionalFormatting sqref="D8:D55">
     <cfRule type="dataBar" priority="47">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8351,12 +8038,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BF6:BK58 I6:AW58 AY6:BD58 BM6:BR58 BT6:BY58 CA6:CF58 CH6:CM58">
+  <conditionalFormatting sqref="BF6:BK55 I6:AW55 AY6:BD55 BM6:BR55 BT6:BY55 CA6:CF55 CH6:CM55">
     <cfRule type="expression" dxfId="8" priority="66">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BF8:BK58 I8:AW58 AY8:BD58 BM8:BR58 BT8:BY58 CA8:CF58 CH8:CM58">
+  <conditionalFormatting sqref="BF8:BK55 I8:AW55 AY8:BD55 BM8:BR55 BT8:BY55 CA8:CF55 CH8:CM55">
     <cfRule type="expression" dxfId="7" priority="60">
       <formula>AND(task_start&lt;=I$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$6)</formula>
     </cfRule>
@@ -8364,12 +8051,12 @@
       <formula>AND(task_end&gt;=I$6,task_start&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL6:BL58 BE6:BE58 BS6:BS58 BZ6:BZ58 CG6:CG58 CN6:CN58">
+  <conditionalFormatting sqref="BL6:BL55 BE6:BE55 BS6:BS55 BZ6:BZ55 CG6:CG55 CN6:CN55">
     <cfRule type="expression" dxfId="5" priority="76">
       <formula>AND(TODAY()&gt;=BE$6,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL8:BL58 BE8:BE58 BS8:BS58 BZ8:BZ58 CG8:CG58 CN8:CN58">
+  <conditionalFormatting sqref="BL8:BL55 BE8:BE55 BS8:BS55 BZ8:BZ55 CG8:CG55 CN8:CN55">
     <cfRule type="expression" dxfId="4" priority="77">
       <formula>AND(task_start&lt;=BE$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BE$6)</formula>
     </cfRule>
@@ -8377,12 +8064,12 @@
       <formula>AND(task_end&gt;=BE$6,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AX6:AX58">
+  <conditionalFormatting sqref="AX6:AX55">
     <cfRule type="expression" dxfId="2" priority="81">
       <formula>AND(TODAY()&gt;=AX$6,TODAY()&lt;BF$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AX8:AX58">
+  <conditionalFormatting sqref="AX8:AX55">
     <cfRule type="expression" dxfId="1" priority="86">
       <formula>AND(task_start&lt;=AX$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AX$6)</formula>
     </cfRule>
@@ -8421,7 +8108,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D8:D58</xm:sqref>
+          <xm:sqref>D8:D55</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8533,23 +8220,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8841,22 +8517,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8883,9 +8566,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>